<commit_message>
will plot logarithmic scale
</commit_message>
<xml_diff>
--- a/sabah/Chapter01/Chapter01.xlsx
+++ b/sabah/Chapter01/Chapter01.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="185">
   <si>
     <r>
       <t>V</t>
@@ -2209,15 +2209,23 @@
       <t>a</t>
     </r>
   </si>
+  <si>
+    <t>vD</t>
+  </si>
+  <si>
+    <t>iD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
     <numFmt numFmtId="165" formatCode="0.000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="33" x14ac:knownFonts="1">
     <font>
@@ -2775,7 +2783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2883,6 +2891,15 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -4215,11 +4232,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1424353168"/>
-        <c:axId val="-1424350992"/>
+        <c:axId val="-1750832912"/>
+        <c:axId val="-1794113600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1424353168"/>
+        <c:axId val="-1750832912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4230,7 +4247,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424350992"/>
+        <c:crossAx val="-1794113600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4240,7 +4257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1424350992"/>
+        <c:axId val="-1794113600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0000000000000002E-2"/>
@@ -4252,7 +4269,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1424353168"/>
+        <c:crossAx val="-1750832912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4276,6 +4293,1147 @@
     <c:pageSetup paperSize="9" orientation="landscape" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'P1.1.3-1.1.5'!$I$34:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P1.1.3-1.1.5'!$J$34:$J$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.949593433094285E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6443347521892064E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6607631597690245E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1319366527409099E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1371695375704625E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4616772976802726E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0000194959343309E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.8420547988619308E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6813133893643728E-2</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.000">
+                  <c:v>0.32029439190669523</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.000">
+                  <c:v>2.1914472398708376</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.000">
+                  <c:v>14.993834525500707</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'P1.1.3-1.1.5'!$I$34:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P1.1.3-1.1.5'!$K$34:$K$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.949593433094285E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0581469443822234E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0727649250935908E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1823751758647181E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8552200233512447E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0961895221934238E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.772378585787237E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0889631773935964E-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.7684981331087092E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0896334612172773E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.7725159859076349E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0910941059893418E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'P1.1.3-1.1.5'!$I$34:$I$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'P1.1.3-1.1.5'!$L$34:$L$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.949593433094285E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.524589605789358E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6443347521892064E-8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8420424475786924E-7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6607631597690245E-7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2033740424362703E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1319366527409099E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1765117387458909E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1371695375704625E-5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.588656892691798E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4616772976802726E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.8231774754874612E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1507052352"/>
+        <c:axId val="-1507050176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1507052352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1507050176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="2"/>
+        <c:tickMarkSkip val="2"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1507050176"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1507052352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9207,23 +10365,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -9231,6 +10376,36 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>376990</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>160421</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>545432</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>72190</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Диаграмма 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -17106,10 +18281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N29"/>
+  <dimension ref="A2:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17117,7 +18292,11 @@
     <col min="5" max="5" width="8.109375" customWidth="1"/>
     <col min="6" max="6" width="3.44140625" customWidth="1"/>
     <col min="7" max="7" width="5.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
@@ -17402,6 +18581,250 @@
       <c r="C29" t="s">
         <v>60</v>
       </c>
+    </row>
+    <row r="30" spans="2:13" ht="18" x14ac:dyDescent="0.4">
+      <c r="J30" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30">
+        <v>9.747967165471425E-9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I32" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="J32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I33" s="2"/>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>1.67</v>
+      </c>
+      <c r="L33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I34" s="2">
+        <v>0</v>
+      </c>
+      <c r="J34" s="69">
+        <f>$K$30*(EXP($I34/(J$33*$B$4))+1)</f>
+        <v>1.949593433094285E-8</v>
+      </c>
+      <c r="K34" s="69">
+        <f>$K$30*(EXP($I34/(K$33*$B$4))+1)</f>
+        <v>1.949593433094285E-8</v>
+      </c>
+      <c r="L34" s="69">
+        <f>$K$30*(EXP($I34/(L$33*$B$4))+1)</f>
+        <v>1.949593433094285E-8</v>
+      </c>
+      <c r="M34" s="71"/>
+    </row>
+    <row r="35" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I35" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="J35" s="69">
+        <f>$K$30*(EXP($I35/(J$33*$B$4))+1)</f>
+        <v>7.6443347521892064E-8</v>
+      </c>
+      <c r="K35" s="69">
+        <f>$K$30*(EXP($I35/(K$33*$B$4))+1)</f>
+        <v>4.0581469443822234E-8</v>
+      </c>
+      <c r="L35" s="69">
+        <f>$K$30*(EXP($I35/(L$33*$B$4))+1)</f>
+        <v>3.524589605789358E-8</v>
+      </c>
+      <c r="M35" s="71"/>
+    </row>
+    <row r="36" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I36" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="J36" s="69">
+        <f>$K$30*(EXP($I36/(J$33*$B$4))+1)</f>
+        <v>4.6607631597690245E-7</v>
+      </c>
+      <c r="K36" s="69">
+        <f>$K$30*(EXP($I36/(K$33*$B$4))+1)</f>
+        <v>1.0727649250935908E-7</v>
+      </c>
+      <c r="L36" s="69">
+        <f>$K$30*(EXP($I36/(L$33*$B$4))+1)</f>
+        <v>7.6443347521892064E-8</v>
+      </c>
+      <c r="M36" s="71"/>
+    </row>
+    <row r="37" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I37" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="J37" s="69">
+        <f>$K$30*(EXP($I37/(J$33*$B$4))+1)</f>
+        <v>3.1319366527409099E-6</v>
+      </c>
+      <c r="K37" s="69">
+        <f>$K$30*(EXP($I37/(K$33*$B$4))+1)</f>
+        <v>3.1823751758647181E-7</v>
+      </c>
+      <c r="L37" s="69">
+        <f>$K$30*(EXP($I37/(L$33*$B$4))+1)</f>
+        <v>1.8420424475786924E-7</v>
+      </c>
+      <c r="M37" s="71"/>
+    </row>
+    <row r="38" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I38" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J38" s="69">
+        <f>$K$30*(EXP($I38/(J$33*$B$4))+1)</f>
+        <v>2.1371695375704625E-5</v>
+      </c>
+      <c r="K38" s="69">
+        <f>$K$30*(EXP($I38/(K$33*$B$4))+1)</f>
+        <v>9.8552200233512447E-7</v>
+      </c>
+      <c r="L38" s="69">
+        <f>$K$30*(EXP($I38/(L$33*$B$4))+1)</f>
+        <v>4.6607631597690245E-7</v>
+      </c>
+      <c r="M38" s="71"/>
+    </row>
+    <row r="39" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I39" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J39" s="69">
+        <f>$K$30*(EXP($I39/(J$33*$B$4))+1)</f>
+        <v>1.4616772976802726E-4</v>
+      </c>
+      <c r="K39" s="69">
+        <f>$K$30*(EXP($I39/(K$33*$B$4))+1)</f>
+        <v>3.0961895221934238E-6</v>
+      </c>
+      <c r="L39" s="69">
+        <f>$K$30*(EXP($I39/(L$33*$B$4))+1)</f>
+        <v>1.2033740424362703E-6</v>
+      </c>
+      <c r="M39" s="71"/>
+    </row>
+    <row r="40" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I40" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="J40" s="69">
+        <f>$K$30*(EXP($I40/(J$33*$B$4))+1)</f>
+        <v>1.0000194959343309E-3</v>
+      </c>
+      <c r="K40" s="69">
+        <f>$K$30*(EXP($I40/(K$33*$B$4))+1)</f>
+        <v>9.772378585787237E-6</v>
+      </c>
+      <c r="L40" s="69">
+        <f>$K$30*(EXP($I40/(L$33*$B$4))+1)</f>
+        <v>3.1319366527409099E-6</v>
+      </c>
+      <c r="M40" s="71"/>
+    </row>
+    <row r="41" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I41" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="J41" s="69">
+        <f>$K$30*(EXP($I41/(J$33*$B$4))+1)</f>
+        <v>6.8420547988619308E-3</v>
+      </c>
+      <c r="K41" s="69">
+        <f>$K$30*(EXP($I41/(K$33*$B$4))+1)</f>
+        <v>3.0889631773935964E-5</v>
+      </c>
+      <c r="L41" s="69">
+        <f>$K$30*(EXP($I41/(L$33*$B$4))+1)</f>
+        <v>8.1765117387458909E-6</v>
+      </c>
+      <c r="M41" s="71"/>
+    </row>
+    <row r="42" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I42" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="J42" s="69">
+        <f>$K$30*(EXP($I42/(J$33*$B$4))+1)</f>
+        <v>4.6813133893643728E-2</v>
+      </c>
+      <c r="K42" s="69">
+        <f>$K$30*(EXP($I42/(K$33*$B$4))+1)</f>
+        <v>9.7684981331087092E-5</v>
+      </c>
+      <c r="L42" s="69">
+        <f>$K$30*(EXP($I42/(L$33*$B$4))+1)</f>
+        <v>2.1371695375704625E-5</v>
+      </c>
+      <c r="M42" s="71"/>
+    </row>
+    <row r="43" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I43" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="J43" s="70">
+        <f>$K$30*(EXP($I43/(J$33*$B$4))+1)</f>
+        <v>0.32029439190669523</v>
+      </c>
+      <c r="K43" s="69">
+        <f>$K$30*(EXP($I43/(K$33*$B$4))+1)</f>
+        <v>3.0896334612172773E-4</v>
+      </c>
+      <c r="L43" s="69">
+        <f>$K$30*(EXP($I43/(L$33*$B$4))+1)</f>
+        <v>5.588656892691798E-5</v>
+      </c>
+      <c r="M43" s="71"/>
+    </row>
+    <row r="44" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I44" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J44" s="70">
+        <f>$K$30*(EXP($I44/(J$33*$B$4))+1)</f>
+        <v>2.1914472398708376</v>
+      </c>
+      <c r="K44" s="69">
+        <f>$K$30*(EXP($I44/(K$33*$B$4))+1)</f>
+        <v>9.7725159859076349E-4</v>
+      </c>
+      <c r="L44" s="69">
+        <f>$K$30*(EXP($I44/(L$33*$B$4))+1)</f>
+        <v>1.4616772976802726E-4</v>
+      </c>
+      <c r="M44" s="71"/>
+    </row>
+    <row r="45" spans="9:13" x14ac:dyDescent="0.3">
+      <c r="I45" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J45" s="70">
+        <f>$K$30*(EXP($I45/(J$33*$B$4))+1)</f>
+        <v>14.993834525500707</v>
+      </c>
+      <c r="K45" s="69">
+        <f>$K$30*(EXP($I45/(K$33*$B$4))+1)</f>
+        <v>3.0910941059893418E-3</v>
+      </c>
+      <c r="L45" s="69">
+        <f>$K$30*(EXP($I45/(L$33*$B$4))+1)</f>
+        <v>3.8231774754874612E-4</v>
+      </c>
+      <c r="M45" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>